<commit_message>
Adding the full json template
</commit_message>
<xml_diff>
--- a/data/all_sports.xlsx
+++ b/data/all_sports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphonsusteow/Documents/alph_projects/SportSG/CodeProjects/major_games_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B5135B-2913-EE4A-9B4F-3CA71A12FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89521CF0-5E7B-FB40-9FC1-3DE264462335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34700" yWindow="660" windowWidth="38080" windowHeight="20780" activeTab="3" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="20220" activeTab="5" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="major_games_future_feature" sheetId="12" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8223" uniqueCount="2066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8282" uniqueCount="2066">
   <si>
     <t>*</t>
   </si>
@@ -7223,7 +7223,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7260,12 +7260,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF2E2F30"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
@@ -7280,7 +7274,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -7301,15 +7295,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -7337,15 +7322,15 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -27498,8 +27483,8 @@
   </sheetPr>
   <dimension ref="A3:B299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E302" sqref="E302"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27533,7 +27518,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>1184</v>
       </c>
       <c r="B6">
@@ -27541,7 +27526,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>1175</v>
       </c>
       <c r="B7">
@@ -27565,7 +27550,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>1050</v>
       </c>
       <c r="B10">
@@ -27573,7 +27558,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>1041</v>
       </c>
       <c r="B11">
@@ -27581,7 +27566,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>1055</v>
       </c>
       <c r="B12">
@@ -27589,7 +27574,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>1060</v>
       </c>
       <c r="B13">
@@ -27605,7 +27590,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="10" t="s">
         <v>1041</v>
       </c>
       <c r="B15">
@@ -27629,7 +27614,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="10" t="s">
         <v>1638</v>
       </c>
       <c r="B18">
@@ -27653,7 +27638,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="10" t="s">
         <v>1574</v>
       </c>
       <c r="B21">
@@ -27661,7 +27646,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="10" t="s">
         <v>1590</v>
       </c>
       <c r="B22">
@@ -27669,7 +27654,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="10" t="s">
         <v>1569</v>
       </c>
       <c r="B23">
@@ -27677,7 +27662,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="10" t="s">
         <v>1581</v>
       </c>
       <c r="B24">
@@ -27693,7 +27678,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="10" t="s">
         <v>1574</v>
       </c>
       <c r="B26">
@@ -27717,7 +27702,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B29">
@@ -27733,7 +27718,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B31">
@@ -27749,7 +27734,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B33">
@@ -27765,7 +27750,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B35">
@@ -27781,7 +27766,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B37">
@@ -27789,7 +27774,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B38">
@@ -27813,7 +27798,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B41">
@@ -27829,7 +27814,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B43">
@@ -27837,7 +27822,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B44">
@@ -27861,7 +27846,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B47">
@@ -27885,7 +27870,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="10" t="s">
         <v>911</v>
       </c>
       <c r="B50">
@@ -27901,7 +27886,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="10" t="s">
         <v>906</v>
       </c>
       <c r="B52">
@@ -27909,7 +27894,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="10" t="s">
         <v>911</v>
       </c>
       <c r="B53">
@@ -27925,7 +27910,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="10" t="s">
         <v>911</v>
       </c>
       <c r="B55">
@@ -27941,7 +27926,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="10" t="s">
         <v>906</v>
       </c>
       <c r="B57">
@@ -27965,7 +27950,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="10" t="s">
         <v>1270</v>
       </c>
       <c r="B60">
@@ -27981,7 +27966,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="10" t="s">
         <v>1255</v>
       </c>
       <c r="B62">
@@ -27989,7 +27974,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="10" t="s">
         <v>1265</v>
       </c>
       <c r="B63">
@@ -27997,7 +27982,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="10" t="s">
         <v>1260</v>
       </c>
       <c r="B64">
@@ -28013,7 +27998,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="10" t="s">
         <v>1270</v>
       </c>
       <c r="B66">
@@ -28021,7 +28006,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="10" t="s">
         <v>1265</v>
       </c>
       <c r="B67">
@@ -28029,7 +28014,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="10" t="s">
         <v>1275</v>
       </c>
       <c r="B68">
@@ -28053,7 +28038,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="10" t="s">
         <v>1316</v>
       </c>
       <c r="B71">
@@ -28069,7 +28054,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="10" t="s">
         <v>1308</v>
       </c>
       <c r="B73">
@@ -28085,7 +28070,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="13" t="s">
+      <c r="A75" s="10" t="s">
         <v>1316</v>
       </c>
       <c r="B75">
@@ -28093,7 +28078,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="10" t="s">
         <v>1303</v>
       </c>
       <c r="B76">
@@ -28101,7 +28086,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="10" t="s">
         <v>1308</v>
       </c>
       <c r="B77">
@@ -28125,7 +28110,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="10" t="s">
         <v>1497</v>
       </c>
       <c r="B80">
@@ -28133,7 +28118,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="10" t="s">
         <v>1492</v>
       </c>
       <c r="B81">
@@ -28141,7 +28126,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="10" t="s">
         <v>1487</v>
       </c>
       <c r="B82">
@@ -28149,7 +28134,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="10" t="s">
         <v>1504</v>
       </c>
       <c r="B83">
@@ -28173,7 +28158,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="10" t="s">
         <v>889</v>
       </c>
       <c r="B86">
@@ -28181,7 +28166,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="10" t="s">
         <v>902</v>
       </c>
       <c r="B87">
@@ -28189,7 +28174,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="10" t="s">
         <v>899</v>
       </c>
       <c r="B88">
@@ -28205,7 +28190,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="10" t="s">
         <v>889</v>
       </c>
       <c r="B90">
@@ -28221,7 +28206,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="10" t="s">
         <v>889</v>
       </c>
       <c r="B92">
@@ -28245,7 +28230,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="10" t="s">
         <v>1663</v>
       </c>
       <c r="B95">
@@ -28253,7 +28238,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="10" t="s">
         <v>1668</v>
       </c>
       <c r="B96">
@@ -28269,7 +28254,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="10" t="s">
         <v>1654</v>
       </c>
       <c r="B98">
@@ -28285,7 +28270,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="10" t="s">
         <v>1654</v>
       </c>
       <c r="B100">
@@ -28309,7 +28294,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="10" t="s">
         <v>1465</v>
       </c>
       <c r="B103">
@@ -28317,7 +28302,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="13" t="s">
+      <c r="A104" s="10" t="s">
         <v>1478</v>
       </c>
       <c r="B104">
@@ -28333,7 +28318,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="13" t="s">
+      <c r="A106" s="10" t="s">
         <v>1465</v>
       </c>
       <c r="B106">
@@ -28341,7 +28326,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="10" t="s">
         <v>1483</v>
       </c>
       <c r="B107">
@@ -28365,7 +28350,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="13" t="s">
+      <c r="A110" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B110">
@@ -28381,7 +28366,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="13" t="s">
+      <c r="A112" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B112">
@@ -28397,7 +28382,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="13" t="s">
+      <c r="A114" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B114">
@@ -28421,7 +28406,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="13" t="s">
+      <c r="A117" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B117">
@@ -28437,7 +28422,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="13" t="s">
+      <c r="A119" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B119">
@@ -28453,7 +28438,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B121">
@@ -28477,7 +28462,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="13" t="s">
+      <c r="A124" s="10" t="s">
         <v>996</v>
       </c>
       <c r="B124">
@@ -28493,7 +28478,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="13" t="s">
+      <c r="A126" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B126">
@@ -28509,7 +28494,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="13" t="s">
+      <c r="A128" s="10" t="s">
         <v>996</v>
       </c>
       <c r="B128">
@@ -28533,7 +28518,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="13" t="s">
+      <c r="A131" s="10" t="s">
         <v>850</v>
       </c>
       <c r="B131">
@@ -28549,7 +28534,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="13" t="s">
+      <c r="A133" s="10" t="s">
         <v>850</v>
       </c>
       <c r="B133">
@@ -28565,7 +28550,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="13" t="s">
+      <c r="A135" s="10" t="s">
         <v>850</v>
       </c>
       <c r="B135">
@@ -28589,7 +28574,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="13" t="s">
+      <c r="A138" s="10" t="s">
         <v>1119</v>
       </c>
       <c r="B138">
@@ -28605,7 +28590,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="13" t="s">
+      <c r="A140" s="10" t="s">
         <v>1119</v>
       </c>
       <c r="B140">
@@ -28629,7 +28614,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="10" t="s">
         <v>1444</v>
       </c>
       <c r="B143">
@@ -28645,7 +28630,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="13" t="s">
+      <c r="A145" s="10" t="s">
         <v>1444</v>
       </c>
       <c r="B145">
@@ -28669,7 +28654,7 @@
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="13" t="s">
+      <c r="A148" s="10" t="s">
         <v>1554</v>
       </c>
       <c r="B148">
@@ -28685,7 +28670,7 @@
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="13" t="s">
+      <c r="A150" s="10" t="s">
         <v>1544</v>
       </c>
       <c r="B150">
@@ -28693,7 +28678,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="13" t="s">
+      <c r="A151" s="10" t="s">
         <v>1549</v>
       </c>
       <c r="B151">
@@ -28701,7 +28686,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="13" t="s">
+      <c r="A152" s="10" t="s">
         <v>1564</v>
       </c>
       <c r="B152">
@@ -28709,7 +28694,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="13" t="s">
+      <c r="A153" s="10" t="s">
         <v>1559</v>
       </c>
       <c r="B153">
@@ -28733,7 +28718,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="13" t="s">
+      <c r="A156" s="10" t="s">
         <v>1333</v>
       </c>
       <c r="B156">
@@ -28749,7 +28734,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="13" t="s">
+      <c r="A158" s="10" t="s">
         <v>1333</v>
       </c>
       <c r="B158">
@@ -28757,7 +28742,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="13" t="s">
+      <c r="A159" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B159">
@@ -28773,7 +28758,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="13" t="s">
+      <c r="A161" s="10" t="s">
         <v>1347</v>
       </c>
       <c r="B161">
@@ -28789,7 +28774,7 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="13" t="s">
+      <c r="A163" s="10" t="s">
         <v>1342</v>
       </c>
       <c r="B163">
@@ -28813,7 +28798,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="13" t="s">
+      <c r="A166" s="10" t="s">
         <v>1596</v>
       </c>
       <c r="B166">
@@ -28829,7 +28814,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="13" t="s">
+      <c r="A168" s="10" t="s">
         <v>1596</v>
       </c>
       <c r="B168">
@@ -28845,7 +28830,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="13" t="s">
+      <c r="A170" s="10" t="s">
         <v>1596</v>
       </c>
       <c r="B170">
@@ -28861,7 +28846,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="13" t="s">
+      <c r="A172" s="10" t="s">
         <v>1596</v>
       </c>
       <c r="B172">
@@ -28885,7 +28870,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="13" t="s">
+      <c r="A175" s="10" t="s">
         <v>879</v>
       </c>
       <c r="B175">
@@ -28893,7 +28878,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="13" t="s">
+      <c r="A176" s="10" t="s">
         <v>1113</v>
       </c>
       <c r="B176">
@@ -28901,7 +28886,7 @@
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="13" t="s">
+      <c r="A177" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="B177">
@@ -28925,7 +28910,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="13" t="s">
+      <c r="A180" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B180">
@@ -28941,7 +28926,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="13" t="s">
+      <c r="A182" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B182">
@@ -28957,7 +28942,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="13" t="s">
+      <c r="A184" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B184">
@@ -28981,7 +28966,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="13" t="s">
+      <c r="A187" s="10" t="s">
         <v>1225</v>
       </c>
       <c r="B187">
@@ -28989,7 +28974,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="13" t="s">
+      <c r="A188" s="10" t="s">
         <v>1215</v>
       </c>
       <c r="B188">
@@ -28997,7 +28982,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="13" t="s">
+      <c r="A189" s="10" t="s">
         <v>1233</v>
       </c>
       <c r="B189">
@@ -29005,7 +28990,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="13" t="s">
+      <c r="A190" s="10" t="s">
         <v>1229</v>
       </c>
       <c r="B190">
@@ -29021,7 +29006,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="13" t="s">
+      <c r="A192" s="10" t="s">
         <v>1220</v>
       </c>
       <c r="B192">
@@ -29045,7 +29030,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="13" t="s">
+      <c r="A195" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B195">
@@ -29061,7 +29046,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="13" t="s">
+      <c r="A197" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B197">
@@ -29069,7 +29054,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="13" t="s">
+      <c r="A198" s="10" t="s">
         <v>874</v>
       </c>
       <c r="B198">
@@ -29085,7 +29070,7 @@
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="13" t="s">
+      <c r="A200" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B200">
@@ -29093,7 +29078,7 @@
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="13" t="s">
+      <c r="A201" s="10" t="s">
         <v>874</v>
       </c>
       <c r="B201">
@@ -29101,7 +29086,7 @@
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="13" t="s">
+      <c r="A202" s="10" t="s">
         <v>879</v>
       </c>
       <c r="B202">
@@ -29117,7 +29102,7 @@
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="13" t="s">
+      <c r="A204" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B204">
@@ -29141,7 +29126,7 @@
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="13" t="s">
+      <c r="A207" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B207">
@@ -29157,7 +29142,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="13" t="s">
+      <c r="A209" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B209">
@@ -29165,7 +29150,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="13" t="s">
+      <c r="A210" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B210">
@@ -29181,7 +29166,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="13" t="s">
+      <c r="A212" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B212">
@@ -29197,7 +29182,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="13" t="s">
+      <c r="A214" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B214">
@@ -29221,7 +29206,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="13" t="s">
+      <c r="A217" s="10" t="s">
         <v>1428</v>
       </c>
       <c r="B217">
@@ -29237,7 +29222,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="13" t="s">
+      <c r="A219" s="10" t="s">
         <v>1410</v>
       </c>
       <c r="B219">
@@ -29245,7 +29230,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="13" t="s">
+      <c r="A220" s="10" t="s">
         <v>1423</v>
       </c>
       <c r="B220">
@@ -29253,7 +29238,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="13" t="s">
+      <c r="A221" s="10" t="s">
         <v>1420</v>
       </c>
       <c r="B221">
@@ -29261,7 +29246,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="13" t="s">
+      <c r="A222" s="10" t="s">
         <v>1415</v>
       </c>
       <c r="B222">
@@ -29269,7 +29254,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="13" t="s">
+      <c r="A223" s="10" t="s">
         <v>1428</v>
       </c>
       <c r="B223">
@@ -29285,7 +29270,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="13" t="s">
+      <c r="A225" s="10" t="s">
         <v>1428</v>
       </c>
       <c r="B225">
@@ -29301,7 +29286,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="13" t="s">
+      <c r="A227" s="10" t="s">
         <v>1428</v>
       </c>
       <c r="B227">
@@ -29325,7 +29310,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="13" t="s">
+      <c r="A230" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B230">
@@ -29341,7 +29326,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="13" t="s">
+      <c r="A232" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B232">
@@ -29357,7 +29342,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="13" t="s">
+      <c r="A234" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B234">
@@ -29365,7 +29350,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A235" s="13" t="s">
+      <c r="A235" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B235">
@@ -29373,7 +29358,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A236" s="13" t="s">
+      <c r="A236" s="10" t="s">
         <v>978</v>
       </c>
       <c r="B236">
@@ -29397,7 +29382,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A239" s="13" t="s">
+      <c r="A239" s="10" t="s">
         <v>861</v>
       </c>
       <c r="B239">
@@ -29405,7 +29390,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A240" s="13" t="s">
+      <c r="A240" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B240">
@@ -29421,7 +29406,7 @@
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A242" s="13" t="s">
+      <c r="A242" s="10" t="s">
         <v>1028</v>
       </c>
       <c r="B242">
@@ -29445,7 +29430,7 @@
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A245" s="13" t="s">
+      <c r="A245" s="10" t="s">
         <v>951</v>
       </c>
       <c r="B245">
@@ -29453,7 +29438,7 @@
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A246" s="13" t="s">
+      <c r="A246" s="10" t="s">
         <v>964</v>
       </c>
       <c r="B246">
@@ -29469,7 +29454,7 @@
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A248" s="13" t="s">
+      <c r="A248" s="10" t="s">
         <v>964</v>
       </c>
       <c r="B248">
@@ -29485,7 +29470,7 @@
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A250" s="13" t="s">
+      <c r="A250" s="10" t="s">
         <v>964</v>
       </c>
       <c r="B250">
@@ -29509,7 +29494,7 @@
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A253" s="13" t="s">
+      <c r="A253" s="10" t="s">
         <v>1357</v>
       </c>
       <c r="B253">
@@ -29517,7 +29502,7 @@
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A254" s="13" t="s">
+      <c r="A254" s="10" t="s">
         <v>145</v>
       </c>
       <c r="B254">
@@ -29525,7 +29510,7 @@
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A255" s="13" t="s">
+      <c r="A255" s="10" t="s">
         <v>143</v>
       </c>
       <c r="B255">
@@ -29541,7 +29526,7 @@
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A257" s="13" t="s">
+      <c r="A257" s="10" t="s">
         <v>1357</v>
       </c>
       <c r="B257">
@@ -29565,7 +29550,7 @@
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A260" s="13" t="s">
+      <c r="A260" s="10" t="s">
         <v>926</v>
       </c>
       <c r="B260">
@@ -29581,7 +29566,7 @@
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A262" s="13" t="s">
+      <c r="A262" s="10" t="s">
         <v>926</v>
       </c>
       <c r="B262">
@@ -29597,7 +29582,7 @@
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A264" s="13" t="s">
+      <c r="A264" s="10" t="s">
         <v>926</v>
       </c>
       <c r="B264">
@@ -29613,7 +29598,7 @@
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A266" s="13" t="s">
+      <c r="A266" s="10" t="s">
         <v>926</v>
       </c>
       <c r="B266">
@@ -29629,7 +29614,7 @@
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A268" s="13" t="s">
+      <c r="A268" s="10" t="s">
         <v>926</v>
       </c>
       <c r="B268">
@@ -29653,7 +29638,7 @@
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A271" s="13" t="s">
+      <c r="A271" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="B271">
@@ -29669,7 +29654,7 @@
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" s="13" t="s">
+      <c r="A273" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="B273">
@@ -29685,7 +29670,7 @@
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" s="13" t="s">
+      <c r="A275" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="B275">
@@ -29701,7 +29686,7 @@
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" s="13" t="s">
+      <c r="A277" s="10" t="s">
         <v>1064</v>
       </c>
       <c r="B277">
@@ -29725,7 +29710,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" s="13" t="s">
+      <c r="A280" s="10" t="s">
         <v>1297</v>
       </c>
       <c r="B280">
@@ -29733,7 +29718,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" s="13" t="s">
+      <c r="A281" s="10" t="s">
         <v>1287</v>
       </c>
       <c r="B281">
@@ -29741,7 +29726,7 @@
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" s="13" t="s">
+      <c r="A282" s="10" t="s">
         <v>1292</v>
       </c>
       <c r="B282">
@@ -29765,7 +29750,7 @@
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" s="13" t="s">
+      <c r="A285" s="10" t="s">
         <v>1534</v>
       </c>
       <c r="B285">
@@ -29773,7 +29758,7 @@
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" s="13" t="s">
+      <c r="A286" s="10" t="s">
         <v>1510</v>
       </c>
       <c r="B286">
@@ -29789,7 +29774,7 @@
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" s="13" t="s">
+      <c r="A288" s="10" t="s">
         <v>1519</v>
       </c>
       <c r="B288">
@@ -29805,7 +29790,7 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="13" t="s">
+      <c r="A290" s="10" t="s">
         <v>1527</v>
       </c>
       <c r="B290">
@@ -29829,7 +29814,7 @@
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" s="13" t="s">
+      <c r="A293" s="10" t="s">
         <v>1169</v>
       </c>
       <c r="B293">
@@ -29837,7 +29822,7 @@
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" s="13" t="s">
+      <c r="A294" s="10" t="s">
         <v>1164</v>
       </c>
       <c r="B294">
@@ -29845,7 +29830,7 @@
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A295" s="13" t="s">
+      <c r="A295" s="10" t="s">
         <v>1156</v>
       </c>
       <c r="B295">
@@ -29863,7 +29848,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A298" s="13" t="s">
+      <c r="A298" s="10" t="s">
         <v>1673</v>
       </c>
     </row>
@@ -29887,8 +29872,8 @@
   </sheetPr>
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35089,890 +35074,891 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
         <v>1679</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>1800</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="11" t="s">
         <v>1782</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="11" t="s">
         <v>1791</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="11" t="s">
         <v>1798</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
         <v>1797</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="12" t="s">
         <v>845</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="11" t="s">
         <v>1680</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="11" t="s">
         <v>1812</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="12" t="s">
         <v>1681</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="12" t="s">
         <v>1801</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="13" t="s">
         <v>1682</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="12" t="s">
         <v>1684</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="12" t="s">
         <v>1799</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="12" t="s">
         <v>1785</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="11" t="s">
         <v>1801</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="12" t="s">
         <v>1683</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="12" t="s">
         <v>1061</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="12" t="s">
         <v>2015</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="12" t="s">
         <v>1685</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>1785</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="12" t="s">
         <v>1794</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="12" t="s">
         <v>1678</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="12" t="s">
         <v>1044</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>1820</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="12" t="s">
         <v>1795</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="12" t="s">
         <v>1818</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="12" t="s">
         <v>1792</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="12" t="s">
         <v>1802</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="12" t="s">
         <v>1785</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="12" t="s">
         <v>1806</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="12" t="s">
         <v>1803</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>1804</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="12" t="s">
         <v>1785</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="12" t="s">
         <v>1794</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="12" t="s">
         <v>1801</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="12" t="s">
         <v>1807</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="12" t="s">
         <v>1044</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>1805</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="12" t="s">
         <v>1795</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="12" t="s">
         <v>1808</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="12" t="s">
         <v>1651</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="12" t="s">
         <v>1814</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="12" t="s">
         <v>1795</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="12" t="s">
         <v>1801</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="12" t="s">
         <v>1801</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="12" t="s">
         <v>1811</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="12" t="s">
         <v>1646</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="12" t="s">
         <v>1809</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="12" t="s">
         <v>1786</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="12" t="s">
         <v>1810</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="12" t="s">
         <v>1593</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="12" t="s">
         <v>1813</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="12" t="s">
         <v>1846</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="12" t="s">
         <v>1815</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="12" t="s">
         <v>1816</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="12" t="s">
         <v>1827</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="12" t="s">
         <v>1821</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="12" t="s">
         <v>1819</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="12" t="s">
         <v>1823</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="12" t="s">
         <v>1387</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="12" t="s">
         <v>1825</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="12" t="s">
         <v>1822</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="12" t="s">
         <v>1826</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="12" t="s">
         <v>1399</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="12" t="s">
         <v>2005</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="12" t="s">
         <v>2007</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="12" t="s">
         <v>2006</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="12" t="s">
         <v>1847</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="12" t="s">
         <v>1827</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="12" t="s">
         <v>1837</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="12" t="s">
         <v>1796</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="12" t="s">
         <v>1838</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="12" t="s">
         <v>1839</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>2008</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="12" t="s">
         <v>1840</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="12" t="s">
         <v>1842</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="12" t="s">
         <v>1841</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="12" t="s">
         <v>1844</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="12" t="s">
         <v>1843</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="12" t="s">
         <v>1845</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="12" t="s">
         <v>1150</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="12" t="s">
         <v>2010</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="12" t="s">
         <v>1840</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="12" t="s">
         <v>2009</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="12" t="s">
         <v>2011</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="12" t="s">
         <v>2015</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>2019</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="12" t="s">
         <v>2012</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="12" t="s">
         <v>1793</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="13" t="s">
         <v>2014</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="12" t="s">
         <v>1495</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="12" t="s">
         <v>2015</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>2020</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="12" t="s">
         <v>2007</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="12" t="s">
         <v>2021</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="12" t="s">
         <v>1847</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="12" t="s">
         <v>1827</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="12" t="s">
         <v>2023</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="11" t="s">
         <v>1784</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="11" t="s">
         <v>2037</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="11" t="s">
         <v>1677</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>2024</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="12" t="s">
         <v>1666</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="12" t="s">
         <v>2031</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="11" t="s">
         <v>2030</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="11" t="s">
         <v>2025</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="12" t="s">
         <v>2026</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="12" t="s">
         <v>1657</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="12" t="s">
         <v>2032</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="12" t="s">
         <v>2038</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="11" t="s">
         <v>1784</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="11" t="s">
         <v>1793</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="12" t="s">
         <v>2039</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="12" t="s">
         <v>2041</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="11" t="s">
         <v>1784</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="11" t="s">
         <v>2007</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="12" t="s">
         <v>2042</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="12" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="12" t="s">
         <v>2043</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="12" t="s">
         <v>2007</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="12" t="s">
         <v>2044</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="12" t="s">
         <v>1100</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="12" t="s">
         <v>2045</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="11" t="s">
         <v>1784</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="11" t="s">
         <v>2007</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="12" t="s">
         <v>2046</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="12" t="s">
         <v>1104</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="12" t="s">
         <v>2050</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="11" t="s">
         <v>2047</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="11" t="s">
         <v>2048</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="12" t="s">
         <v>2049</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="12" t="s">
         <v>1236</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="12" t="s">
         <v>2054</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="11" t="s">
         <v>2053</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="11" t="s">
         <v>2007</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="11" t="s">
         <v>1676</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="11" t="s">
         <v>1677</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="12" t="s">
         <v>2055</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="12" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="12" t="s">
         <v>2064</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="12" t="s">
         <v>1677</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="12" t="s">
         <v>1784</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="12" t="s">
         <v>2007</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="12" t="s">
         <v>1676</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="12" t="s">
         <v>2063</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="12" t="s">
         <v>2065</v>
       </c>
     </row>
@@ -35990,7 +35976,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36187,10 +36173,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:C288"/>
+  <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="117" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36199,7 +36185,7 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>839</v>
       </c>
@@ -36209,8 +36195,11 @@
       <c r="C1" t="s">
         <v>1782</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1357</v>
       </c>
@@ -36220,8 +36209,11 @@
       <c r="C2" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -36231,8 +36223,11 @@
       <c r="C3" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -36242,8 +36237,11 @@
       <c r="C4" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1357</v>
       </c>
@@ -36253,8 +36251,11 @@
       <c r="C5" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -36264,8 +36265,11 @@
       <c r="C6" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -36275,8 +36279,11 @@
       <c r="C7" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -36286,8 +36293,11 @@
       <c r="C8" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -36297,8 +36307,11 @@
       <c r="C9" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -36308,8 +36321,11 @@
       <c r="C10" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -36319,8 +36335,11 @@
       <c r="C11" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -36330,8 +36349,11 @@
       <c r="C12" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -36341,8 +36363,11 @@
       <c r="C13" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -36352,8 +36377,11 @@
       <c r="C14" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -36363,8 +36391,11 @@
       <c r="C15" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -36374,8 +36405,11 @@
       <c r="C16" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -36385,8 +36419,11 @@
       <c r="C17" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -36396,8 +36433,11 @@
       <c r="C18" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -36407,8 +36447,11 @@
       <c r="C19" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -36418,8 +36461,11 @@
       <c r="C20" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -36429,8 +36475,11 @@
       <c r="C21" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -36440,8 +36489,11 @@
       <c r="C22" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -36451,8 +36503,11 @@
       <c r="C23" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -36462,8 +36517,11 @@
       <c r="C24" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -36473,8 +36531,11 @@
       <c r="C25" t="s">
         <v>1786</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -36484,8 +36545,11 @@
       <c r="C26" t="s">
         <v>1786</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -36495,8 +36559,11 @@
       <c r="C27" t="s">
         <v>1786</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -36506,8 +36573,11 @@
       <c r="C28" t="s">
         <v>1786</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -36517,8 +36587,11 @@
       <c r="C29" t="s">
         <v>1787</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -36528,8 +36601,11 @@
       <c r="C30" t="s">
         <v>1787</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -36539,8 +36615,11 @@
       <c r="C31" t="s">
         <v>1787</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -36550,8 +36629,11 @@
       <c r="C32" t="s">
         <v>1787</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -36561,8 +36643,11 @@
       <c r="C33" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -36572,8 +36657,11 @@
       <c r="C34" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -36583,8 +36671,11 @@
       <c r="C35" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -36594,8 +36685,11 @@
       <c r="C36" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -36605,8 +36699,11 @@
       <c r="C37" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -36616,8 +36713,11 @@
       <c r="C38" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -36627,8 +36727,11 @@
       <c r="C39" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -36638,8 +36741,11 @@
       <c r="C40" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -36649,8 +36755,11 @@
       <c r="C41" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -36660,8 +36769,11 @@
       <c r="C42" t="s">
         <v>1785</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -36671,8 +36783,11 @@
       <c r="C43" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -36682,8 +36797,11 @@
       <c r="C44" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>27</v>
       </c>
@@ -36693,8 +36811,11 @@
       <c r="C45" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>27</v>
       </c>
@@ -36704,8 +36825,11 @@
       <c r="C46" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -36715,8 +36839,11 @@
       <c r="C47" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -36726,8 +36853,11 @@
       <c r="C48" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -36737,8 +36867,11 @@
       <c r="C49" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -36748,8 +36881,11 @@
       <c r="C50" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -36759,8 +36895,11 @@
       <c r="C51" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -36770,16 +36909,25 @@
       <c r="C52" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -36789,8 +36937,11 @@
       <c r="C54" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -36800,8 +36951,11 @@
       <c r="C55" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -36811,8 +36965,11 @@
       <c r="C56" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -36822,8 +36979,11 @@
       <c r="C57" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>34</v>
       </c>
@@ -36833,8 +36993,11 @@
       <c r="C58" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -36844,8 +37007,11 @@
       <c r="C59" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -36856,7 +37022,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -36867,7 +37033,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -36878,7 +37044,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -36889,7 +37055,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -39374,776 +39540,689 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="140.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>408</v>
       </c>
       <c r="B1" t="s">
         <v>1737</v>
       </c>
-      <c r="C1" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>1692</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1765</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>1756</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>1757</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>1758</v>
       </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>1759</v>
       </c>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>1760</v>
       </c>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>1761</v>
       </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>1762</v>
       </c>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>1763</v>
       </c>
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>1567</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>1764</v>
       </c>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>1693</v>
       </c>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>1695</v>
       </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>1696</v>
       </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>1738</v>
       </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>1739</v>
       </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>1697</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>1698</v>
       </c>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>1699</v>
       </c>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>1700</v>
       </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>1740</v>
       </c>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>1701</v>
       </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>1702</v>
       </c>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>1741</v>
       </c>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>1703</v>
       </c>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>1704</v>
       </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>1705</v>
       </c>
-      <c r="C31" s="9"/>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>1742</v>
       </c>
-      <c r="C32" s="9"/>
-    </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C33" s="9"/>
-    </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C34" s="9"/>
-    </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>1743</v>
       </c>
-      <c r="C36" s="9"/>
-    </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>1706</v>
       </c>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>1707</v>
       </c>
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>1708</v>
       </c>
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C40" s="9"/>
-    </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>1744</v>
       </c>
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>1745</v>
       </c>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>1746</v>
       </c>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>1709</v>
       </c>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>108</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>1710</v>
       </c>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>1711</v>
       </c>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>111</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>1712</v>
       </c>
-      <c r="C48" s="9"/>
-    </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>1713</v>
       </c>
-      <c r="C49" s="9"/>
-    </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>1714</v>
       </c>
-      <c r="C50" s="9"/>
-    </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>1715</v>
       </c>
-      <c r="C51" s="9"/>
-    </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>118</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>1716</v>
       </c>
-      <c r="C52" s="9"/>
-    </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>120</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>1717</v>
       </c>
-      <c r="C53" s="9"/>
-    </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>122</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>1718</v>
       </c>
-      <c r="C54" s="9"/>
-    </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>125</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>1719</v>
       </c>
-      <c r="C55" s="9"/>
-    </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>1747</v>
       </c>
-      <c r="C56" s="9"/>
-    </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>133</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C57" s="9"/>
-    </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>1720</v>
       </c>
-      <c r="C58" s="9"/>
-    </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>135</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>1721</v>
       </c>
-      <c r="C59" s="9"/>
-    </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1722</v>
       </c>
       <c r="B60" t="s">
         <v>1748</v>
       </c>
-      <c r="C60" s="9"/>
-    </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1722</v>
       </c>
       <c r="B61" t="s">
         <v>1749</v>
       </c>
-      <c r="C61" s="9"/>
-    </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1722</v>
       </c>
       <c r="B62" t="s">
         <v>1750</v>
       </c>
-      <c r="C62" s="9"/>
-    </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1722</v>
       </c>
       <c r="B63" t="s">
         <v>1751</v>
       </c>
-      <c r="C63" s="9"/>
-    </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1722</v>
       </c>
       <c r="B64" t="s">
         <v>1752</v>
       </c>
-      <c r="C64" s="9"/>
-    </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1722</v>
       </c>
       <c r="B65" t="s">
         <v>1753</v>
       </c>
-      <c r="C65" s="9"/>
-    </row>
-    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1722</v>
       </c>
       <c r="B66" t="s">
         <v>1754</v>
       </c>
-      <c r="C66" s="9"/>
-    </row>
-    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1722</v>
       </c>
       <c r="B67" t="s">
         <v>1755</v>
       </c>
-      <c r="C67" s="9"/>
-    </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>1723</v>
       </c>
-      <c r="C68" s="9"/>
-    </row>
-    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="9" t="s">
         <v>1724</v>
       </c>
-      <c r="C69" s="9"/>
-    </row>
-    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>141</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>1725</v>
       </c>
-      <c r="C70" s="9"/>
-    </row>
-    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>142</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="9" t="s">
         <v>1726</v>
       </c>
-      <c r="C71" s="9"/>
-    </row>
-    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>143</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="9" t="s">
         <v>1727</v>
       </c>
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>146</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="9" t="s">
         <v>1728</v>
       </c>
-      <c r="C73" s="9"/>
-    </row>
-    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>147</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>1729</v>
       </c>
-      <c r="C74" s="9"/>
-    </row>
-    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C75" s="9"/>
-    </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="9" t="s">
         <v>1730</v>
       </c>
-      <c r="C76" s="9"/>
-    </row>
-    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>154</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="9" t="s">
         <v>1731</v>
       </c>
-      <c r="C77" s="9"/>
-    </row>
-    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B78" s="9" t="s">
         <v>1732</v>
       </c>
-      <c r="C78" s="9"/>
-    </row>
-    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B79" s="9" t="s">
         <v>1733</v>
       </c>
-      <c r="C79" s="9"/>
-    </row>
-    <row r="80" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>159</v>
       </c>
-      <c r="B80" s="10" t="s">
+      <c r="B80" s="9" t="s">
         <v>1734</v>
       </c>
-      <c r="C80" s="9"/>
-    </row>
-    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="9" t="s">
         <v>1735</v>
       </c>
-      <c r="C81" s="9"/>
-    </row>
-    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>242</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="B82" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C82" s="9"/>
-    </row>
-    <row r="83" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>268</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B83" s="9" t="s">
         <v>1694</v>
       </c>
-      <c r="C83" s="9"/>
-    </row>
-    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>388</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="9" t="s">
         <v>1736</v>
       </c>
-      <c r="C84" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40363,7 +40442,7 @@
   <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding the new mapping system
</commit_message>
<xml_diff>
--- a/data/all_sports.xlsx
+++ b/data/all_sports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphonsusteow/Documents/alph_projects/SportSG/CodeProjects/major_games_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89521CF0-5E7B-FB40-9FC1-3DE264462335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EB1D7F-0668-424C-BE23-F0E34BAD065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="20220" activeTab="5" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
+    <workbookView xWindow="34720" yWindow="660" windowWidth="18960" windowHeight="20780" activeTab="3" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="major_games_future_feature" sheetId="12" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7129,94 +7129,94 @@
     <t xml:space="preserve">GOLF </t>
   </si>
   <si>
+    <t>["GENDER", "ROUND", "NAME", "SCORE", "PAR_STATUS", "TOTAL_PARTICIPANTS"]</t>
+  </si>
+  <si>
+    <t>*{SPORT} - {GENDER} {EVENT_NAME} {ROUND}*
+{ATHLETE1} (SGP) VS {ATHLETE2} ({COUNTRY2})
+Score: {SCORE}. {WINNER} beat {LOSER} and {ADVANCEMENT_STATUS}, which will be held on {DATE} at {TIME} ({HOST_COUNTRY_CODE} time).</t>
+  </si>
+  <si>
+    <t>["SPORT", "GENDER", "EVENT_NAME", "ATHLETE1", "ATHLETE2", "COUNTRY2", "SCORE", "WINNER", "LOSER", "ADVANCEMENT_STATUS",  "DATE", "TIME"]</t>
+  </si>
+  <si>
+    <t>*PENCAK SILAT - MEN REGU QUARTER FINALS*
+TEAM OF {ATHLETE1}, {ATHLETE2} &amp; {ATHLETE3} (SGP) VS TEAM OF {ATHLETE4}, {ATHLETE5} &amp; {ATHLETE6} ({COUNTRY1})
+Score: {SCORE}. {WINNER} beat {LOSER}. SGP {ADVANCEMENT_STATUS}.</t>
+  </si>
+  <si>
+    <t>["ATHLETE1", "ATHLETE2", "ATHLETE3", "ATHLETE4", "ATHLETE5", "ATHLETE6", "SCORE", "WINNER", "LOSER", "ADVANCEMENT_STATUS"]</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>fleet racing day</t>
+  </si>
+  <si>
+    <t>["SPORT", "GENDER", "EVENT_NAME", "ROUND", "ROUND_NO", "NAME", "POINTS", "RANK", "TOTAL", "RACES"]</t>
+  </si>
+  <si>
+    <t>*{SPORT} -{GENDER} {EVENT_NAME} {ROUND} {ROUND_NO}*
+{NAME} (SGP)
+Total Points: {POINTS}. Currently ranked {RANK} out of {TOTAL} after {RACES} races.</t>
+  </si>
+  <si>
+    <t>"NEXT_ROUND", "NEXT_DATE", "TIME", "HOST_COUNTRY_CODE"</t>
+  </si>
+  <si>
+    <t>Round {NEXT_ROUND} will be held on {NEXT_DATE} at {TIME} ({HOST_COUNTRY_CODE} time).</t>
+  </si>
+  <si>
+    <t>combined time</t>
+  </si>
+  <si>
+    <t>*{SPORT} - {GENDER} {CREWS} CREWS ({AGE_CAT}) {EVENT_NAME} {ROUND} {ROUND_NUMBER}*
+Time: {TIME}
+SGP finished {PLACEMENT} out of {TOTAL}. With a combined time of {COMBINED_TIME}, SGP finished {OVERALL_PLACEMENT} overall.</t>
+  </si>
+  <si>
+    <t>["SPORT", "GENDER", "CREWS", "AGE_CAT",  "EVENT_NAME", "ROUND", "ROUND_NUMBER", "TIME", "PLACEMENT", "TOTAL", "COMBINED_TIME", "OVERALL_PLACEMENT"]</t>
+  </si>
+  <si>
+    <t>RELAY</t>
+  </si>
+  <si>
+    <t>CHANGQUAN</t>
+  </si>
+  <si>
+    <t>DAOSHU</t>
+  </si>
+  <si>
+    <t>GUNSHU</t>
+  </si>
+  <si>
+    <t>DUILIAN</t>
+  </si>
+  <si>
+    <t>TAIJIQUAN</t>
+  </si>
+  <si>
+    <t>TAIJIJIAN</t>
+  </si>
+  <si>
+    <t>["SPORT", "GENDER", "EVENT1", "EVENT2", "ROUND", "EVENT_CAT", "NAME", "SCORE", "PLACEMENT", "TOTAL", "NEXT_EVENT", "DATE", "TIME", "HOST_COUNTRY_CODE"]</t>
+  </si>
+  <si>
+    <t>*{SPORT} - {GENDER} {EVENT1} + {EVENT2} {ROUND} (EVENT_CAT)*
+{NAME}
+Score: {SCORE}. Finished {PLACEMENT} out of {TOTAL} and will be competing in {NEXT_EVENT} on {DATE} at {TIME} ({HOST_COUNTRY_CODE}  time).</t>
+  </si>
+  <si>
+    <t>*WUSHU MEN TAIJIQUAN + TAIJIJIAN COMBINED FINALS (TAIJIQUAN)*
+{NAME}
+Score: {SCORE}. Finished {PLACEMENT} out of {TOTAL} and will be competing in Tajijian on {DATE} at {TIME} (CAM time).</t>
+  </si>
+  <si>
     <t>*GOLF - {GENDER} {EVENT_NAME} {ROUND}*
 {NAME} (SGP)
 Individual Score of {SCORE} ({PAR_STATUS})
-She is currently ranked {RANK} out of {TOTAL_PARTICIPANTS} after {ROUND}.</t>
-  </si>
-  <si>
-    <t>["GENDER", "ROUND", "NAME", "SCORE", "PAR_STATUS", "TOTAL_PARTICIPANTS"]</t>
-  </si>
-  <si>
-    <t>*{SPORT} - {GENDER} {EVENT_NAME} {ROUND}*
-{ATHLETE1} (SGP) VS {ATHLETE2} ({COUNTRY2})
-Score: {SCORE}. {WINNER} beat {LOSER} and {ADVANCEMENT_STATUS}, which will be held on {DATE} at {TIME} ({HOST_COUNTRY_CODE} time).</t>
-  </si>
-  <si>
-    <t>["SPORT", "GENDER", "EVENT_NAME", "ATHLETE1", "ATHLETE2", "COUNTRY2", "SCORE", "WINNER", "LOSER", "ADVANCEMENT_STATUS",  "DATE", "TIME"]</t>
-  </si>
-  <si>
-    <t>*PENCAK SILAT - MEN REGU QUARTER FINALS*
-TEAM OF {ATHLETE1}, {ATHLETE2} &amp; {ATHLETE3} (SGP) VS TEAM OF {ATHLETE4}, {ATHLETE5} &amp; {ATHLETE6} ({COUNTRY1})
-Score: {SCORE}. {WINNER} beat {LOSER}. SGP {ADVANCEMENT_STATUS}.</t>
-  </si>
-  <si>
-    <t>["ATHLETE1", "ATHLETE2", "ATHLETE3", "ATHLETE4", "ATHLETE5", "ATHLETE6", "SCORE", "WINNER", "LOSER", "ADVANCEMENT_STATUS"]</t>
-  </si>
-  <si>
-    <t>points</t>
-  </si>
-  <si>
-    <t>fleet racing day</t>
-  </si>
-  <si>
-    <t>["SPORT", "GENDER", "EVENT_NAME", "ROUND", "ROUND_NO", "NAME", "POINTS", "RANK", "TOTAL", "RACES"]</t>
-  </si>
-  <si>
-    <t>*{SPORT} -{GENDER} {EVENT_NAME} {ROUND} {ROUND_NO}*
-{NAME} (SGP)
-Total Points: {POINTS}. Currently ranked {RANK} out of {TOTAL} after {RACES} races.</t>
-  </si>
-  <si>
-    <t>"NEXT_ROUND", "NEXT_DATE", "TIME", "HOST_COUNTRY_CODE"</t>
-  </si>
-  <si>
-    <t>Round {NEXT_ROUND} will be held on {NEXT_DATE} at {TIME} ({HOST_COUNTRY_CODE} time).</t>
-  </si>
-  <si>
-    <t>combined time</t>
-  </si>
-  <si>
-    <t>*{SPORT} - {GENDER} {CREWS} CREWS ({AGE_CAT}) {EVENT_NAME} {ROUND} {ROUND_NUMBER}*
-Time: {TIME}
-SGP finished {PLACEMENT} out of {TOTAL}. With a combined time of {COMBINED_TIME}, SGP finished {OVERALL_PLACEMENT} overall.</t>
-  </si>
-  <si>
-    <t>["SPORT", "GENDER", "CREWS", "AGE_CAT",  "EVENT_NAME", "ROUND", "ROUND_NUMBER", "TIME", "PLACEMENT", "TOTAL", "COMBINED_TIME", "OVERALL_PLACEMENT"]</t>
-  </si>
-  <si>
-    <t>RELAY</t>
-  </si>
-  <si>
-    <t>CHANGQUAN</t>
-  </si>
-  <si>
-    <t>DAOSHU</t>
-  </si>
-  <si>
-    <t>GUNSHU</t>
-  </si>
-  <si>
-    <t>DUILIAN</t>
-  </si>
-  <si>
-    <t>TAIJIQUAN</t>
-  </si>
-  <si>
-    <t>TAIJIJIAN</t>
-  </si>
-  <si>
-    <t>["SPORT", "GENDER", "EVENT1", "EVENT2", "ROUND", "EVENT_CAT", "NAME", "SCORE", "PLACEMENT", "TOTAL", "NEXT_EVENT", "DATE", "TIME", "HOST_COUNTRY_CODE"]</t>
-  </si>
-  <si>
-    <t>*{SPORT} - {GENDER} {EVENT1} + {EVENT2} {ROUND} (EVENT_CAT)*
-{NAME}
-Score: {SCORE}. Finished {PLACEMENT} out of {TOTAL} and will be competing in {NEXT_EVENT} on {DATE} at {TIME} ({HOST_COUNTRY_CODE}  time).</t>
-  </si>
-  <si>
-    <t>*WUSHU MEN TAIJIQUAN + TAIJIJIAN COMBINED FINALS (TAIJIQUAN)*
-{NAME}
-Score: {SCORE}. Finished {PLACEMENT} out of {TOTAL} and will be competing in Tajijian on {DATE} at {TIME} (CAM time).</t>
+Is currently ranked {RANK} out of {TOTAL_PARTICIPANTS} after {ROUND}.</t>
   </si>
 </sst>
 </file>
@@ -7301,7 +7301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7325,11 +7325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9738,7 +9734,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF0C7554-B27A-0C48-960B-F75D2A192274}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF0C7554-B27A-0C48-960B-F75D2A192274}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B299" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -35074,896 +35070,900 @@
   </sheetPr>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" t="s">
         <v>1679</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" t="s">
         <v>844</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" t="s">
         <v>1800</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" t="s">
         <v>1782</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" t="s">
         <v>1791</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" t="s">
         <v>1798</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" t="s">
         <v>1797</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="5" t="s">
         <v>845</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" t="s">
         <v>1680</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" t="s">
         <v>1812</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    <row r="2" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>2026</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>1657</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1809</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1786</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1810</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>1593</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>2014</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>1495</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>26</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>2048</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>2006</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1847</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>2041</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2042</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>2043</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>2062</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B10" s="5" t="s">
         <v>1681</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D10" s="5" t="s">
         <v>1784</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E10" s="5" t="s">
         <v>1793</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F10" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G10" s="5" t="s">
         <v>1801</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H10" s="11" t="s">
         <v>1682</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I10" s="5" t="s">
         <v>1684</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="11">
+    <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>1815</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1816</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>2039</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2037</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>2024</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>1826</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>1806</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>1678</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>2053</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>2054</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>2021</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>1847</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>2045</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>1842</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>2011</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1845</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>1819</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>1823</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>1820</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>1818</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>1808</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>1811</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>1646</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>1838</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B29" s="5" t="s">
         <v>1799</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C29" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D29" s="5" t="s">
         <v>1785</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E29" s="5" t="s">
         <v>1793</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F29" t="s">
         <v>1676</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G29" t="s">
         <v>1801</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H29" s="5" t="s">
         <v>1683</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I29" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J29" s="5" t="s">
         <v>2015</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>1794</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>1678</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>1820</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>1818</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>1802</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>1806</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>1804</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>1794</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>1801</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>1807</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>1805</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>1808</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>1651</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>1801</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>1801</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>1811</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>1646</v>
-      </c>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>1809</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>1786</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>1810</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>1593</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>1813</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>1846</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>1815</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>1816</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>1819</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>1823</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>1825</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>1822</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>1826</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>2005</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>2006</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>1847</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>1837</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>1796</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>1838</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>2008</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>1842</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>1844</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>1845</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>2010</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>2009</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>2011</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>2019</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>2012</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>2014</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>1495</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>2020</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>2021</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>1847</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="11">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>2023</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>2037</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>2024</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>21</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>2031</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>2030</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>2025</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>2026</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>1657</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>2032</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23" s="11">
-        <v>22</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>2038</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>2039</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="11">
-        <v>23</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>2041</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>2042</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
-        <v>24</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>2043</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>2044</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A26" s="11">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>2045</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>2046</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A27" s="11">
-        <v>26</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>2050</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>2047</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>2048</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>2049</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" s="11">
-        <v>27</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>2054</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>2053</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>2055</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A29" s="11">
-        <v>28</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>2064</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>2063</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>2065</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J28" xr:uid="{5ECE6884-912D-5F43-9F8A-9072DBF917B5}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J29">
+    <sortCondition ref="C2:C29"/>
+    <sortCondition ref="D2:D29"/>
+    <sortCondition ref="E2:E29"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -36035,10 +36035,10 @@
         <v>1817</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -36175,7 +36175,7 @@
   </sheetPr>
   <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="117" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="117" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -36246,7 +36246,7 @@
         <v>1357</v>
       </c>
       <c r="B5" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C5" t="s">
         <v>1785</v>
@@ -36260,7 +36260,7 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C6" t="s">
         <v>1785</v>
@@ -36274,7 +36274,7 @@
         <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C7" t="s">
         <v>1785</v>
@@ -39469,7 +39469,7 @@
         <v>159</v>
       </c>
       <c r="B283" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="C283" t="s">
         <v>1784</v>
@@ -39480,7 +39480,7 @@
         <v>159</v>
       </c>
       <c r="B284" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="C284" t="s">
         <v>1784</v>
@@ -39491,7 +39491,7 @@
         <v>159</v>
       </c>
       <c r="B285" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="C285" t="s">
         <v>1784</v>
@@ -39502,7 +39502,7 @@
         <v>159</v>
       </c>
       <c r="B286" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="C286" t="s">
         <v>1784</v>
@@ -39513,7 +39513,7 @@
         <v>159</v>
       </c>
       <c r="B287" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="C287" t="s">
         <v>1784</v>
@@ -39524,7 +39524,7 @@
         <v>159</v>
       </c>
       <c r="B288" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="C288" t="s">
         <v>1784</v>

</xml_diff>

<commit_message>
Change to use template type and not template raw
</commit_message>
<xml_diff>
--- a/data/all_sports.xlsx
+++ b/data/all_sports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alphonsusteow/Documents/alph_projects/SportSG/CodeProjects/major_games_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EB1D7F-0668-424C-BE23-F0E34BAD065C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D941BA-EFE3-5443-B1DA-F1D2AC9D5087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34720" yWindow="660" windowWidth="18960" windowHeight="20780" activeTab="3" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
+    <workbookView xWindow="17780" yWindow="940" windowWidth="16640" windowHeight="21260" firstSheet="1" activeTab="3" xr2:uid="{B3FB6ABA-A16E-4DC7-8BDC-DC32712CC2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="major_games_future_feature" sheetId="12" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="country_code" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">template_raw!$A$1:$H$199</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">template_type!$A$1:$J$28</definedName>
     <definedName name="tablecode">#REF!</definedName>
   </definedNames>
@@ -29863,13 +29864,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461321B4-46EA-424A-8894-EF226E944BE7}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="F193" sqref="F193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29910,7 +29911,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>847</v>
       </c>
@@ -29936,7 +29937,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>847</v>
       </c>
@@ -29962,7 +29963,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>847</v>
       </c>
@@ -29988,7 +29989,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>859</v>
       </c>
@@ -30014,7 +30015,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>859</v>
       </c>
@@ -30040,7 +30041,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>859</v>
       </c>
@@ -30066,7 +30067,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>859</v>
       </c>
@@ -30092,7 +30093,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>859</v>
       </c>
@@ -30118,7 +30119,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>859</v>
       </c>
@@ -30144,7 +30145,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>859</v>
       </c>
@@ -30170,7 +30171,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>859</v>
       </c>
@@ -30196,7 +30197,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>886</v>
       </c>
@@ -30222,7 +30223,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>886</v>
       </c>
@@ -30248,7 +30249,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>886</v>
       </c>
@@ -30274,7 +30275,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>886</v>
       </c>
@@ -30300,7 +30301,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>886</v>
       </c>
@@ -30326,7 +30327,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>904</v>
       </c>
@@ -30352,7 +30353,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>904</v>
       </c>
@@ -30378,7 +30379,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>904</v>
       </c>
@@ -30404,7 +30405,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>904</v>
       </c>
@@ -30430,7 +30431,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>904</v>
       </c>
@@ -30456,7 +30457,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>924</v>
       </c>
@@ -30482,7 +30483,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>924</v>
       </c>
@@ -30508,7 +30509,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>924</v>
       </c>
@@ -30534,7 +30535,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>924</v>
       </c>
@@ -30560,7 +30561,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>924</v>
       </c>
@@ -30586,7 +30587,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>924</v>
       </c>
@@ -30612,7 +30613,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>949</v>
       </c>
@@ -30638,7 +30639,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>949</v>
       </c>
@@ -30664,7 +30665,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>949</v>
       </c>
@@ -30690,7 +30691,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>949</v>
       </c>
@@ -30716,7 +30717,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>949</v>
       </c>
@@ -30742,7 +30743,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>949</v>
       </c>
@@ -30768,7 +30769,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>949</v>
       </c>
@@ -30794,7 +30795,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>976</v>
       </c>
@@ -30820,7 +30821,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>976</v>
       </c>
@@ -30846,7 +30847,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>976</v>
       </c>
@@ -30872,7 +30873,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>976</v>
       </c>
@@ -30898,7 +30899,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>994</v>
       </c>
@@ -30924,7 +30925,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>994</v>
       </c>
@@ -30950,7 +30951,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>994</v>
       </c>
@@ -30976,7 +30977,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>994</v>
       </c>
@@ -31002,7 +31003,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>994</v>
       </c>
@@ -31028,7 +31029,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>994</v>
       </c>
@@ -31054,7 +31055,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>1018</v>
       </c>
@@ -31080,7 +31081,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>1018</v>
       </c>
@@ -31106,7 +31107,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1018</v>
       </c>
@@ -31132,7 +31133,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1018</v>
       </c>
@@ -31158,7 +31159,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1018</v>
       </c>
@@ -31184,7 +31185,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1039</v>
       </c>
@@ -31210,7 +31211,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1039</v>
       </c>
@@ -31236,7 +31237,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1039</v>
       </c>
@@ -31262,7 +31263,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1039</v>
       </c>
@@ -31288,7 +31289,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1039</v>
       </c>
@@ -31314,7 +31315,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1062</v>
       </c>
@@ -31340,7 +31341,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1062</v>
       </c>
@@ -31366,7 +31367,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1062</v>
       </c>
@@ -31392,7 +31393,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>1062</v>
       </c>
@@ -31418,7 +31419,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1062</v>
       </c>
@@ -31444,7 +31445,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1082</v>
       </c>
@@ -31470,7 +31471,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1082</v>
       </c>
@@ -31496,7 +31497,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1082</v>
       </c>
@@ -31522,7 +31523,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1095</v>
       </c>
@@ -31548,7 +31549,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1095</v>
       </c>
@@ -31574,7 +31575,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1095</v>
       </c>
@@ -31600,7 +31601,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1095</v>
       </c>
@@ -31626,7 +31627,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1095</v>
       </c>
@@ -31652,7 +31653,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1117</v>
       </c>
@@ -31678,7 +31679,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1117</v>
       </c>
@@ -31704,7 +31705,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1117</v>
       </c>
@@ -31730,7 +31731,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1117</v>
       </c>
@@ -31756,7 +31757,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1134</v>
       </c>
@@ -31782,7 +31783,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1139</v>
       </c>
@@ -31808,7 +31809,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1134</v>
       </c>
@@ -31834,7 +31835,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1134</v>
       </c>
@@ -31860,7 +31861,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1134</v>
       </c>
@@ -31886,7 +31887,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1154</v>
       </c>
@@ -31912,7 +31913,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1154</v>
       </c>
@@ -31938,7 +31939,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1154</v>
       </c>
@@ -31964,7 +31965,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1154</v>
       </c>
@@ -31990,7 +31991,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1173</v>
       </c>
@@ -32016,7 +32017,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1173</v>
       </c>
@@ -32042,7 +32043,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1173</v>
       </c>
@@ -32068,7 +32069,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1173</v>
       </c>
@@ -32094,7 +32095,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1190</v>
       </c>
@@ -32120,7 +32121,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1190</v>
       </c>
@@ -32146,7 +32147,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1190</v>
       </c>
@@ -32172,7 +32173,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1190</v>
       </c>
@@ -32198,7 +32199,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1190</v>
       </c>
@@ -32224,7 +32225,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1190</v>
       </c>
@@ -32250,7 +32251,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1213</v>
       </c>
@@ -32276,7 +32277,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1213</v>
       </c>
@@ -32302,7 +32303,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>1213</v>
       </c>
@@ -32328,7 +32329,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1213</v>
       </c>
@@ -32354,7 +32355,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1213</v>
       </c>
@@ -32380,7 +32381,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>1237</v>
       </c>
@@ -32406,7 +32407,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>1237</v>
       </c>
@@ -32432,7 +32433,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>1237</v>
       </c>
@@ -32458,7 +32459,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>1237</v>
       </c>
@@ -32484,7 +32485,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>1253</v>
       </c>
@@ -32510,7 +32511,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>1253</v>
       </c>
@@ -32536,7 +32537,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>1253</v>
       </c>
@@ -32562,7 +32563,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>1253</v>
       </c>
@@ -32588,7 +32589,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>1253</v>
       </c>
@@ -32614,7 +32615,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1253</v>
       </c>
@@ -32640,7 +32641,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>1253</v>
       </c>
@@ -32666,7 +32667,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1285</v>
       </c>
@@ -32692,7 +32693,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>1285</v>
       </c>
@@ -32718,7 +32719,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1285</v>
       </c>
@@ -32744,7 +32745,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1301</v>
       </c>
@@ -32770,7 +32771,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1301</v>
       </c>
@@ -32796,7 +32797,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>1301</v>
       </c>
@@ -32822,7 +32823,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>1301</v>
       </c>
@@ -32848,7 +32849,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>1301</v>
       </c>
@@ -32874,7 +32875,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>1301</v>
       </c>
@@ -32900,7 +32901,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>1301</v>
       </c>
@@ -32926,7 +32927,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>1331</v>
       </c>
@@ -32952,7 +32953,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>1331</v>
       </c>
@@ -32978,7 +32979,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>1331</v>
       </c>
@@ -33004,7 +33005,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>1331</v>
       </c>
@@ -33030,7 +33031,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>1331</v>
       </c>
@@ -33056,7 +33057,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>1355</v>
       </c>
@@ -33082,7 +33083,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>1355</v>
       </c>
@@ -33108,7 +33109,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>1355</v>
       </c>
@@ -33134,7 +33135,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>1355</v>
       </c>
@@ -33160,7 +33161,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>1355</v>
       </c>
@@ -33186,7 +33187,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>1355</v>
       </c>
@@ -33212,7 +33213,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>1355</v>
       </c>
@@ -33238,7 +33239,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1355</v>
       </c>
@@ -33264,7 +33265,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1383</v>
       </c>
@@ -33290,7 +33291,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>1383</v>
       </c>
@@ -33316,7 +33317,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>1383</v>
       </c>
@@ -33342,7 +33343,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>1383</v>
       </c>
@@ -33368,7 +33369,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>1383</v>
       </c>
@@ -33394,7 +33395,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>1383</v>
       </c>
@@ -33420,7 +33421,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>1408</v>
       </c>
@@ -33446,7 +33447,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>1408</v>
       </c>
@@ -33472,7 +33473,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>1408</v>
       </c>
@@ -33498,7 +33499,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>1408</v>
       </c>
@@ -33524,7 +33525,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>1408</v>
       </c>
@@ -33550,7 +33551,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1408</v>
       </c>
@@ -33576,7 +33577,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>1408</v>
       </c>
@@ -33602,7 +33603,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>1408</v>
       </c>
@@ -33628,7 +33629,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>1442</v>
       </c>
@@ -33654,7 +33655,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>1442</v>
       </c>
@@ -33680,7 +33681,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>1442</v>
       </c>
@@ -33706,7 +33707,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>1442</v>
       </c>
@@ -33732,7 +33733,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>1442</v>
       </c>
@@ -33758,7 +33759,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>1442</v>
       </c>
@@ -33784,7 +33785,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>1463</v>
       </c>
@@ -33810,7 +33811,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>1463</v>
       </c>
@@ -33836,7 +33837,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>1463</v>
       </c>
@@ -33862,7 +33863,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>1463</v>
       </c>
@@ -33888,7 +33889,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>1463</v>
       </c>
@@ -33914,7 +33915,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>1485</v>
       </c>
@@ -33940,7 +33941,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>1485</v>
       </c>
@@ -33966,7 +33967,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>1485</v>
       </c>
@@ -33992,7 +33993,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>1485</v>
       </c>
@@ -34018,7 +34019,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>1485</v>
       </c>
@@ -34044,7 +34045,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>1485</v>
       </c>
@@ -34070,7 +34071,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>1508</v>
       </c>
@@ -34096,7 +34097,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>1508</v>
       </c>
@@ -34122,7 +34123,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>1508</v>
       </c>
@@ -34148,7 +34149,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>1508</v>
       </c>
@@ -34174,7 +34175,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>1508</v>
       </c>
@@ -34200,7 +34201,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>1508</v>
       </c>
@@ -34226,7 +34227,7 @@
         <v>1532</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>1508</v>
       </c>
@@ -34252,7 +34253,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>1508</v>
       </c>
@@ -34278,7 +34279,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>1542</v>
       </c>
@@ -34304,7 +34305,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>1542</v>
       </c>
@@ -34330,7 +34331,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>1542</v>
       </c>
@@ -34356,7 +34357,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>1542</v>
       </c>
@@ -34382,7 +34383,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>1542</v>
       </c>
@@ -34408,7 +34409,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>1567</v>
       </c>
@@ -34434,7 +34435,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>1567</v>
       </c>
@@ -34460,7 +34461,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>1567</v>
       </c>
@@ -34486,7 +34487,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>1567</v>
       </c>
@@ -34512,7 +34513,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>1567</v>
       </c>
@@ -34538,7 +34539,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>1567</v>
       </c>
@@ -34564,7 +34565,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>1594</v>
       </c>
@@ -34590,7 +34591,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>1594</v>
       </c>
@@ -34616,7 +34617,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>1594</v>
       </c>
@@ -34642,7 +34643,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>1594</v>
       </c>
@@ -34668,7 +34669,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>1612</v>
       </c>
@@ -34694,7 +34695,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1612</v>
       </c>
@@ -34720,7 +34721,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>1612</v>
       </c>
@@ -34746,7 +34747,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>1612</v>
       </c>
@@ -34772,7 +34773,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>1612</v>
       </c>
@@ -34798,7 +34799,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>1612</v>
       </c>
@@ -34954,7 +34955,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>1652</v>
       </c>
@@ -34980,7 +34981,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>1652</v>
       </c>
@@ -35006,7 +35007,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>1652</v>
       </c>
@@ -35032,7 +35033,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1652</v>
       </c>
@@ -35059,6 +35060,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H199" xr:uid="{461321B4-46EA-424A-8894-EF226E944BE7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Aquatics Waterpolo"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -35071,8 +35079,8 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35120,117 +35128,111 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2031</v>
-      </c>
-      <c r="C2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D2" t="s">
-        <v>2030</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2025</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>2026</v>
+      <c r="G2" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1682</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>1657</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>2032</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1809</v>
+        <v>1799</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>1793</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" t="s">
         <v>1676</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>1677</v>
+      <c r="G3" t="s">
+        <v>1801</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>1810</v>
+        <v>1683</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>1593</v>
+        <v>1061</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>1813</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2019</v>
+        <v>1685</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1677</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>2012</v>
+        <v>1785</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F4" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G4" t="s">
         <v>1676</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>2014</v>
+      <c r="H4" s="5" t="s">
+        <v>1678</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>1495</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2049</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2046</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2047</v>
+        <v>1820</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1795</v>
       </c>
       <c r="F5" t="s">
         <v>1677</v>
@@ -35239,143 +35241,141 @@
         <v>1676</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>2048</v>
+        <v>1818</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>2005</v>
+        <v>1802</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>1677</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>2007</v>
+        <v>1793</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
+        <v>1806</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>2006</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>1847</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>23</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>2065</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" s="5" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>1676</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>2041</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>24</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>2042</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>1677</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>1784</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>2007</v>
+        <v>1795</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>1676</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>2043</v>
+        <v>1808</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>1100</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2063</v>
+        <v>1814</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>1784</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>2007</v>
+        <v>1795</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>1676</v>
+        <v>1801</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>1676</v>
+        <v>1801</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>2062</v>
+        <v>1811</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>2064</v>
-      </c>
+        <v>1646</v>
+      </c>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1681</v>
+        <v>1809</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>1677</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>1784</v>
+        <v>1786</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>1793</v>
@@ -35384,13 +35384,16 @@
         <v>1676</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>1801</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>1682</v>
+        <v>1677</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1810</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>1684</v>
+        <v>1593</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>1813</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -35427,68 +35430,68 @@
     </row>
     <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2038</v>
-      </c>
-      <c r="C12" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1819</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D12" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G12" t="s">
-        <v>1677</v>
-      </c>
       <c r="H12" s="5" t="s">
-        <v>2039</v>
+        <v>1823</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>1009</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>2023</v>
-      </c>
-      <c r="C13" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
         <v>1784</v>
       </c>
-      <c r="E13" t="s">
-        <v>2037</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1822</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G13" t="s">
-        <v>1677</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>2024</v>
+        <v>1826</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>1666</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1825</v>
+        <v>2005</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>1677</v>
@@ -35497,7 +35500,7 @@
         <v>1784</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>1822</v>
+        <v>2007</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>1677</v>
@@ -35506,463 +35509,466 @@
         <v>1676</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>1826</v>
+        <v>2006</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>1847</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1802</v>
+        <v>1837</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>1796</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
+        <v>1838</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>1806</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>1794</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="H16" s="5" t="s">
+        <v>1842</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>1677</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>1678</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>1804</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>1794</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>1801</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>1676</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>1807</v>
+        <v>1845</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2053</v>
-      </c>
-      <c r="C18" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="D18" t="s">
-        <v>2052</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D18" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="5" t="s">
         <v>1677</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>2054</v>
+        <v>2009</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>2011</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>2007</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>2021</v>
+      <c r="H19" s="11" t="s">
+        <v>2014</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>1847</v>
+        <v>1495</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>1827</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>2044</v>
-      </c>
-      <c r="C20" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
         <v>1784</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>2007</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="5" t="s">
         <v>1676</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>2045</v>
+        <v>2021</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>1104</v>
+        <v>1847</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>1827</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>2008</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2037</v>
+      </c>
+      <c r="F21" t="s">
         <v>1676</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="G21" t="s">
+        <v>1677</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>2024</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2025</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1676</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>2026</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>1657</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D23" t="s">
         <v>1784</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="E23" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G23" t="s">
         <v>1677</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="H23" s="5" t="s">
+        <v>2039</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C24" t="s">
         <v>1677</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>1842</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>2010</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="D24" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G24" t="s">
         <v>1676</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>2009</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>2011</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>16</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>1844</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>1843</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>1676</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>1845</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>11</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>1676</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>1819</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>1676</v>
-      </c>
       <c r="H24" s="5" t="s">
-        <v>1823</v>
+        <v>2041</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>1387</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>1820</v>
+        <v>2042</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>1784</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F25" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>1677</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="5" t="s">
         <v>1676</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>1818</v>
+        <v>2043</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>1805</v>
-      </c>
-      <c r="C26" s="5" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C26" t="s">
         <v>1676</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" t="s">
         <v>1784</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="E26" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G26" t="s">
         <v>1676</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>1677</v>
-      </c>
       <c r="H26" s="5" t="s">
-        <v>1808</v>
+        <v>2045</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>1651</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C27" s="5" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1677</v>
+      </c>
+      <c r="G27" t="s">
         <v>1676</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>1795</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>1801</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>1801</v>
-      </c>
       <c r="H27" s="5" t="s">
-        <v>1811</v>
+        <v>2048</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>1646</v>
-      </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>1837</v>
-      </c>
-      <c r="C28" s="5" t="s">
+        <v>2053</v>
+      </c>
+      <c r="C28" t="s">
         <v>1676</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>1784</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>1796</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="D28" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1676</v>
+      </c>
+      <c r="G28" t="s">
         <v>1677</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>1676</v>
-      </c>
       <c r="H28" s="5" t="s">
-        <v>1838</v>
+        <v>2054</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>1839</v>
+        <v>962</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>1799</v>
+        <v>2063</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>2007</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>1793</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" s="5" t="s">
         <v>1676</v>
       </c>
-      <c r="G29" t="s">
-        <v>1801</v>
-      </c>
       <c r="H29" s="5" t="s">
-        <v>1683</v>
+        <v>2062</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>1061</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>2015</v>
+        <v>2064</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J28" xr:uid="{5ECE6884-912D-5F43-9F8A-9072DBF917B5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J29">
-    <sortCondition ref="C2:C29"/>
-    <sortCondition ref="D2:D29"/>
-    <sortCondition ref="E2:E29"/>
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39543,7 +39549,7 @@
   <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>